<commit_message>
Redo report on laptop
</commit_message>
<xml_diff>
--- a/scripts/report/jod.xlsx
+++ b/scripts/report/jod.xlsx
@@ -495,25 +495,25 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10.99454610969547</v>
+        <v>7.895089568579725</v>
       </c>
       <c r="E2" t="n">
-        <v>-16.62913696503328</v>
+        <v>-6.674987144438718</v>
       </c>
       <c r="F2" t="n">
-        <v>-3.297777103576925</v>
+        <v>-5.680488882285537</v>
       </c>
       <c r="G2" t="n">
-        <v>-9.882959585112063</v>
+        <v>-6.177742814835656</v>
       </c>
       <c r="H2" t="n">
-        <v>11.73013690122587</v>
+        <v>14.99878708177518</v>
       </c>
       <c r="I2" t="n">
-        <v>3.893162360411909</v>
+        <v>-5.467687944985539</v>
       </c>
       <c r="J2" t="n">
-        <v>3.192015552540177</v>
+        <v>1.107023072538064</v>
       </c>
     </row>
     <row r="3">
@@ -531,25 +531,25 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-6.234286018209565</v>
+        <v>-0.9281962351246827</v>
       </c>
       <c r="E3" t="n">
-        <v>9.974939852339073</v>
+        <v>6.72168738250815</v>
       </c>
       <c r="F3" t="n">
-        <v>0.385065275765029</v>
+        <v>-0.6648559136396395</v>
       </c>
       <c r="G3" t="n">
-        <v>-6.294254537724711</v>
+        <v>-2.027508211865583</v>
       </c>
       <c r="H3" t="n">
-        <v>2.245638499413245</v>
+        <v>0.09793753258278383</v>
       </c>
       <c r="I3" t="n">
-        <v>7.145237956755283</v>
+        <v>-0.4204894376324931</v>
       </c>
       <c r="J3" t="n">
-        <v>-7.222344826288689</v>
+        <v>-2.778578177568736</v>
       </c>
     </row>
     <row r="4">
@@ -567,25 +567,25 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.446036318910741</v>
+        <v>1.446086955100122</v>
       </c>
       <c r="E4" t="n">
-        <v>3.249721891317809</v>
+        <v>3.249772293330987</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.4595598795571639</v>
+        <v>-0.4595092445906481</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09001042499614288</v>
+        <v>0.09006123475212764</v>
       </c>
       <c r="H4" t="n">
-        <v>-7.040936603895439</v>
+        <v>-7.041228894227597</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2885462391115455</v>
+        <v>0.2885967499234481</v>
       </c>
       <c r="J4" t="n">
-        <v>2.426174300620605</v>
+        <v>2.426224687258598</v>
       </c>
     </row>
     <row r="5">
@@ -603,25 +603,25 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-6.84751353474327</v>
+        <v>-6.599612981350536</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.462091159794645</v>
+        <v>-0.1810729435441736</v>
       </c>
       <c r="F5" t="n">
-        <v>-19.79856843504342</v>
+        <v>-20.66456959606492</v>
       </c>
       <c r="G5" t="n">
-        <v>20.47920069785912</v>
+        <v>20.87879642263015</v>
       </c>
       <c r="H5" t="n">
-        <v>13.85642928320215</v>
+        <v>13.80173634841873</v>
       </c>
       <c r="I5" t="n">
-        <v>6.131999541760059</v>
+        <v>6.380599859212127</v>
       </c>
       <c r="J5" t="n">
-        <v>-13.35946395056801</v>
+        <v>-13.61587726669496</v>
       </c>
     </row>
     <row r="6">
@@ -639,25 +639,25 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-4.561665829828817</v>
+        <v>-4.629890234386988</v>
       </c>
       <c r="E6" t="n">
-        <v>9.783924773928751</v>
+        <v>9.353171567705081</v>
       </c>
       <c r="F6" t="n">
-        <v>10.02088736644568</v>
+        <v>10.59986614691645</v>
       </c>
       <c r="G6" t="n">
-        <v>-6.058439267005742</v>
+        <v>-6.126669408505362</v>
       </c>
       <c r="H6" t="n">
-        <v>2.5659205745118</v>
+        <v>2.690645083242104</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.475614777362715</v>
+        <v>-5.54384812702416</v>
       </c>
       <c r="J6" t="n">
-        <v>-6.27506981075226</v>
+        <v>-6.343301974655924</v>
       </c>
     </row>
     <row r="7">
@@ -675,25 +675,25 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-9.411679377775714</v>
+        <v>-6.144925765434117</v>
       </c>
       <c r="E7" t="n">
-        <v>17.42256525551599</v>
+        <v>15.05711507292876</v>
       </c>
       <c r="F7" t="n">
-        <v>-10.399739266202</v>
+        <v>-6.402469829866455</v>
       </c>
       <c r="G7" t="n">
-        <v>3.942883025639432</v>
+        <v>1.241502625342788</v>
       </c>
       <c r="H7" t="n">
-        <v>10.54557047237293</v>
+        <v>7.95501859872583</v>
       </c>
       <c r="I7" t="n">
-        <v>-9.471648086222931</v>
+        <v>-6.341082874346043</v>
       </c>
       <c r="J7" t="n">
-        <v>-2.627979582116981</v>
+        <v>-5.365169809854561</v>
       </c>
     </row>
     <row r="8">
@@ -711,25 +711,25 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-0.216106924285647</v>
+        <v>-0.2161066570902882</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.39996291667523</v>
+        <v>-1.399962587267457</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4449414061947335</v>
+        <v>0.4449416901078789</v>
       </c>
       <c r="G8" t="n">
-        <v>1.377898768602228</v>
+        <v>1.377899017071763</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8905294286875696</v>
+        <v>0.890529759708272</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7764057705532464</v>
+        <v>0.7764060953771168</v>
       </c>
       <c r="J8" t="n">
-        <v>-1.873710626129383</v>
+        <v>-1.873710373508476</v>
       </c>
     </row>
     <row r="9">
@@ -747,25 +747,25 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-11.57191870020881</v>
+        <v>-5.161923432167462</v>
       </c>
       <c r="E9" t="n">
-        <v>10.06434962001704</v>
+        <v>3.372075722868998</v>
       </c>
       <c r="F9" t="n">
-        <v>10.93378081045047</v>
+        <v>5.06877113835789</v>
       </c>
       <c r="G9" t="n">
-        <v>3.317849458453762</v>
+        <v>2.465435716231376</v>
       </c>
       <c r="H9" t="n">
-        <v>10.49907266290191</v>
+        <v>4.203294914274939</v>
       </c>
       <c r="I9" t="n">
-        <v>-4.075566715104157</v>
+        <v>1.884833668745529</v>
       </c>
       <c r="J9" t="n">
-        <v>-19.1675876820439</v>
+        <v>-11.83249446967147</v>
       </c>
     </row>
     <row r="10">
@@ -783,25 +783,25 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-9.519472013198348</v>
+        <v>-3.725993835012948</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.097925158365573</v>
+        <v>-4.183527513374042</v>
       </c>
       <c r="F10" t="n">
-        <v>-3.403893241364262</v>
+        <v>-4.001230094461162</v>
       </c>
       <c r="G10" t="n">
-        <v>3.477391100378444</v>
+        <v>3.060055300550586</v>
       </c>
       <c r="H10" t="n">
-        <v>12.51113347184923</v>
+        <v>9.741603874102358</v>
       </c>
       <c r="I10" t="n">
-        <v>8.037786532999807</v>
+        <v>4.07196193183082</v>
       </c>
       <c r="J10" t="n">
-        <v>-10.00502267583511</v>
+        <v>-4.962874015371635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerun report after weekend
</commit_message>
<xml_diff>
--- a/scripts/report/jod.xlsx
+++ b/scripts/report/jod.xlsx
@@ -495,25 +495,25 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7.895089568579725</v>
+        <v>1.719909931458051</v>
       </c>
       <c r="E2" t="n">
-        <v>-6.674987144438718</v>
+        <v>-0.2039520248260614</v>
       </c>
       <c r="F2" t="n">
-        <v>-5.680488882285537</v>
+        <v>-0.5852272968399153</v>
       </c>
       <c r="G2" t="n">
-        <v>-6.177742814835656</v>
+        <v>-0.7854485348414308</v>
       </c>
       <c r="H2" t="n">
-        <v>14.99878708177518</v>
+        <v>0.6762499159617221</v>
       </c>
       <c r="I2" t="n">
-        <v>-5.467687944985539</v>
+        <v>-0.5436223594072835</v>
       </c>
       <c r="J2" t="n">
-        <v>1.107023072538064</v>
+        <v>-0.2779127231197738</v>
       </c>
     </row>
     <row r="3">
@@ -531,25 +531,25 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-0.9281962351246827</v>
+        <v>0.09903402696768078</v>
       </c>
       <c r="E3" t="n">
-        <v>6.72168738250815</v>
+        <v>1.244516884631022</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.6648559136396395</v>
+        <v>0.3291040908015486</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.027508211865583</v>
+        <v>-1.485789282946316</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09793753258278383</v>
+        <v>0.7868775500378195</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.4204894376324931</v>
+        <v>0.6466933590286569</v>
       </c>
       <c r="J3" t="n">
-        <v>-2.778578177568736</v>
+        <v>-1.620437111431839</v>
       </c>
     </row>
     <row r="4">
@@ -603,25 +603,25 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-6.599612981350536</v>
+        <v>-2.828694456891071</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1810729435441736</v>
+        <v>-3.21069243405172</v>
       </c>
       <c r="F5" t="n">
-        <v>-20.66456959606492</v>
+        <v>-11.20394686822662</v>
       </c>
       <c r="G5" t="n">
-        <v>20.87879642263015</v>
+        <v>12.10898156297891</v>
       </c>
       <c r="H5" t="n">
-        <v>13.80173634841873</v>
+        <v>4.363515621419242</v>
       </c>
       <c r="I5" t="n">
-        <v>6.380599859212127</v>
+        <v>4.363512418870462</v>
       </c>
       <c r="J5" t="n">
-        <v>-13.61587726669496</v>
+        <v>-3.592691926216328</v>
       </c>
     </row>
     <row r="6">
@@ -675,25 +675,25 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-6.144925765434117</v>
+        <v>-1.963586432280363</v>
       </c>
       <c r="E7" t="n">
-        <v>15.05711507292876</v>
+        <v>6.377408859240358</v>
       </c>
       <c r="F7" t="n">
-        <v>-6.402469829866455</v>
+        <v>-2.807264789697831</v>
       </c>
       <c r="G7" t="n">
-        <v>1.241502625342788</v>
+        <v>-1.19844024096829</v>
       </c>
       <c r="H7" t="n">
-        <v>7.95501859872583</v>
+        <v>5.423536811568717</v>
       </c>
       <c r="I7" t="n">
-        <v>-6.341082874346043</v>
+        <v>-2.98686097277585</v>
       </c>
       <c r="J7" t="n">
-        <v>-5.365169809854561</v>
+        <v>-2.844811869253617</v>
       </c>
     </row>
     <row r="8">
@@ -747,25 +747,25 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-5.161923432167462</v>
+        <v>-0.350142292383761</v>
       </c>
       <c r="E9" t="n">
-        <v>3.372075722868998</v>
+        <v>1.453408350316651</v>
       </c>
       <c r="F9" t="n">
-        <v>5.06877113835789</v>
+        <v>2.443275829108928</v>
       </c>
       <c r="G9" t="n">
-        <v>2.465435716231376</v>
+        <v>1.188719351958085</v>
       </c>
       <c r="H9" t="n">
-        <v>4.203294914274939</v>
+        <v>1.823410939967825</v>
       </c>
       <c r="I9" t="n">
-        <v>1.884833668745529</v>
+        <v>0.5515448522164188</v>
       </c>
       <c r="J9" t="n">
-        <v>-11.83249446967147</v>
+        <v>-7.110216070199187</v>
       </c>
     </row>
     <row r="10">
@@ -783,25 +783,25 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-3.725993835012948</v>
+        <v>-0.5086535384326947</v>
       </c>
       <c r="E10" t="n">
-        <v>-4.183527513374042</v>
+        <v>-1.046056444018553</v>
       </c>
       <c r="F10" t="n">
-        <v>-4.001230094461162</v>
+        <v>-0.4541802921307532</v>
       </c>
       <c r="G10" t="n">
-        <v>3.060055300550586</v>
+        <v>2.035443260118563</v>
       </c>
       <c r="H10" t="n">
-        <v>9.741603874102358</v>
+        <v>0.4900824914355656</v>
       </c>
       <c r="I10" t="n">
-        <v>4.07196193183082</v>
+        <v>1.41904260917095</v>
       </c>
       <c r="J10" t="n">
-        <v>-4.962874015371635</v>
+        <v>-1.935680723963911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>